<commit_message>
Ajout de fichiers pour le Scrut
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/Frame/Minimum Rules - Primary Structures.xlsx
+++ b/FR_Frame_Body/Frame/Minimum Rules - Primary Structures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\Gitkraken\STUF2020\STUF-2020\FR_Frame_Body\Frame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08455697-38BC-4375-9887-146F93527C66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4902E464-0423-4806-A191-B39305875AC8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="396" yWindow="684" windowWidth="21468" windowHeight="10872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Etude Structure Primaire" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="36">
   <si>
     <t>Minimum requirements of frame</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Fait par :</t>
   </si>
   <si>
-    <t>v2.0</t>
-  </si>
-  <si>
     <t>Robin CLAMENS</t>
   </si>
   <si>
@@ -132,6 +129,18 @@
   </si>
   <si>
     <t>Catalogue</t>
+  </si>
+  <si>
+    <t>2x + cher que 25x1,5</t>
+  </si>
+  <si>
+    <t>v2.1</t>
+  </si>
+  <si>
+    <t>Véhicule</t>
+  </si>
+  <si>
+    <t>Invictus</t>
   </si>
 </sst>
 </file>
@@ -282,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -385,6 +394,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -938,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1740,7 +1752,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="L33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1754,10 +1766,10 @@
         <v>25</v>
       </c>
       <c r="B60" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" s="23" t="s">
         <v>27</v>
-      </c>
-      <c r="C60" s="23" t="s">
-        <v>28</v>
       </c>
       <c r="D60" s="23"/>
     </row>
@@ -1769,7 +1781,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="23" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B62" s="23"/>
       <c r="C62" s="23"/>
@@ -1777,11 +1789,19 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="24">
-        <v>43690</v>
+        <v>43724</v>
       </c>
       <c r="B63" s="23"/>
       <c r="C63" s="23"/>
       <c r="D63" s="23"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:H33">
@@ -2016,10 +2036,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38401E3-E0D0-4314-90F3-931084C2E20C}">
-  <dimension ref="B3:J41"/>
+  <dimension ref="A3:J41"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2038,10 +2058,10 @@
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
@@ -2225,7 +2245,7 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="27">
         <v>20</v>
@@ -2251,7 +2271,7 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="27">
         <v>20</v>
@@ -2373,7 +2393,7 @@
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B17" s="20"/>
       <c r="C17" s="20">
         <v>24</v>
@@ -2399,7 +2419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B18" s="25" t="s">
         <v>22</v>
       </c>
@@ -2424,7 +2444,7 @@
       <c r="I18" s="6"/>
       <c r="J18" s="25"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B19" s="25" t="s">
         <v>22</v>
       </c>
@@ -2449,9 +2469,12 @@
       <c r="I19" s="25"/>
       <c r="J19" s="25"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="35" t="s">
+        <v>32</v>
+      </c>
       <c r="B20" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="28">
         <v>25</v>
@@ -2477,9 +2500,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B21" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="28">
         <v>25</v>
@@ -2503,7 +2526,7 @@
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B22" s="20"/>
       <c r="C22" s="20">
         <v>26</v>
@@ -2527,7 +2550,7 @@
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B23" s="20"/>
       <c r="C23" s="20">
         <v>26</v>
@@ -2551,7 +2574,7 @@
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B24" s="20"/>
       <c r="C24" s="20">
         <v>27</v>
@@ -2575,7 +2598,7 @@
       <c r="I24" s="20"/>
       <c r="J24" s="22"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B25" s="20"/>
       <c r="C25" s="20">
         <v>27</v>
@@ -2599,7 +2622,7 @@
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B26" s="25" t="s">
         <v>22</v>
       </c>
@@ -2624,7 +2647,7 @@
       <c r="I26" s="7"/>
       <c r="J26" s="25"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B27" s="25" t="s">
         <v>22</v>
       </c>
@@ -2649,9 +2672,9 @@
       <c r="I27" s="25"/>
       <c r="J27" s="25"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B28" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="28">
         <v>28</v>
@@ -2675,9 +2698,9 @@
       <c r="I28" s="25"/>
       <c r="J28" s="25"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B29" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" s="28">
         <v>28</v>
@@ -2701,7 +2724,7 @@
       <c r="I29" s="25"/>
       <c r="J29" s="25"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B30" s="25" t="s">
         <v>22</v>
       </c>
@@ -2726,7 +2749,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="25"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31" s="25" t="s">
         <v>22</v>
       </c>
@@ -2751,9 +2774,9 @@
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="28">
         <v>30</v>

</xml_diff>